<commit_message>
Runmanager xls sheet updated
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -11,11 +11,12 @@
     <sheet name="IterationOptions" sheetId="10" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:E7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -71,7 +72,10 @@
     <t>Verify xpath</t>
   </si>
   <si>
-    <t>True</t>
+    <t>TC_06_Loginpage</t>
+  </si>
+  <si>
+    <t>Login page verification</t>
   </si>
   <si>
     <t>RunAllIterations</t>
@@ -88,9 +92,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -113,28 +117,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,19 +146,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,8 +176,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -181,23 +245,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,50 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -284,55 +288,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,19 +438,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,103 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,34 +500,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,21 +531,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -573,11 +545,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,148 +597,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1119,7 +1123,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="4"/>
@@ -1228,15 +1232,19 @@
         <v>7</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="10"/>
       <c r="E7" s="8"/>
@@ -1275,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" t="b">
         <v>1</v>
@@ -1283,7 +1291,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1291,7 +1299,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>